<commit_message>
Opt TQQQ y pres 10
</commit_message>
<xml_diff>
--- a/Programas e insumos/Optimización parámetros/TQQQ/Fractales.xlsx
+++ b/Programas e insumos/Optimización parámetros/TQQQ/Fractales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDSG\Wissen\GitHub\Swell_2_Optimizacion_estrategias\Programas e insumos\Optimización parámetros\TQQQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c809557\Documents\GitHub\Swell_2_Optimizacion_estrategias\Programas e insumos\Optimización parámetros\TQQQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91319D46-4709-48A1-9AC5-3812DFE9C507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{7CF3DCDF-7C8E-4A43-8556-C04217A46A19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros fractales" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
   <si>
     <t>Estrategia</t>
   </si>
@@ -96,6 +95,9 @@
   </si>
   <si>
     <t>SELL</t>
+  </si>
+  <si>
+    <t>OPEN</t>
   </si>
   <si>
     <t>Función compra</t>
@@ -113,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,12 +463,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE9778-9210-41AC-899F-6D8EA074B69F}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -494,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -576,10 +580,10 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>
@@ -591,57 +595,344 @@
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L3" s="1">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="M3" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
+      <c r="A4" s="1">
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="1">
+        <v>-4</v>
+      </c>
+      <c r="M4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-6</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-3</v>
+      </c>
+      <c r="M7" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="1">
+        <v>-4</v>
+      </c>
+      <c r="M9" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-4</v>
+      </c>
+      <c r="M10" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>